<commit_message>
Actualizacion de carga de alistamiento xlsx
</commit_message>
<xml_diff>
--- a/Files/Temp_alist_adm/_/_.xlsx
+++ b/Files/Temp_alist_adm/_/_.xlsx
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="120">
   <si>
     <t>Guia</t>
   </si>
@@ -1151,9 +1151,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J70" sqref="J70"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P69" sqref="P69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4519,6 +4519,12 @@
       <c r="O60" s="3">
         <v>0</v>
       </c>
+      <c r="P60" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q60" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="R60" s="3" t="s">
         <v>83</v>
       </c>
@@ -4580,6 +4586,12 @@
       <c r="O61" s="3">
         <v>0</v>
       </c>
+      <c r="P61" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q61" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="R61" s="3" t="s">
         <v>83</v>
       </c>
@@ -4641,6 +4653,12 @@
       <c r="O62" s="3">
         <v>0</v>
       </c>
+      <c r="P62" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q62" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="R62" s="3" t="s">
         <v>83</v>
       </c>
@@ -4702,6 +4720,12 @@
       <c r="O63" s="3">
         <v>0</v>
       </c>
+      <c r="P63" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q63" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="R63" s="3" t="s">
         <v>83</v>
       </c>
@@ -4734,7 +4758,7 @@
         <v>101</v>
       </c>
       <c r="F64" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>77</v>
@@ -4762,6 +4786,12 @@
       </c>
       <c r="O64" s="3">
         <v>0</v>
+      </c>
+      <c r="P64" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q64" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="R64" s="3" t="s">
         <v>83</v>
@@ -4795,7 +4825,7 @@
         <v>101</v>
       </c>
       <c r="F65" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>77</v>
@@ -4823,6 +4853,12 @@
       </c>
       <c r="O65" s="3">
         <v>0</v>
+      </c>
+      <c r="P65" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q65" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="R65" s="3" t="s">
         <v>83</v>
@@ -4856,7 +4892,7 @@
         <v>101</v>
       </c>
       <c r="F66" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>77</v>
@@ -4884,6 +4920,12 @@
       </c>
       <c r="O66" s="3">
         <v>0</v>
+      </c>
+      <c r="P66" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q66" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="R66" s="3" t="s">
         <v>83</v>
@@ -4917,7 +4959,7 @@
         <v>101</v>
       </c>
       <c r="F67" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G67" s="3" t="s">
         <v>77</v>
@@ -4945,6 +4987,12 @@
       </c>
       <c r="O67" s="3">
         <v>0</v>
+      </c>
+      <c r="P67" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q67" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="R67" s="3" t="s">
         <v>83</v>
@@ -4978,7 +5026,7 @@
         <v>101</v>
       </c>
       <c r="F68" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>77</v>
@@ -5006,6 +5054,12 @@
       </c>
       <c r="O68" s="3">
         <v>0</v>
+      </c>
+      <c r="P68" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q68" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="R68" s="3" t="s">
         <v>83</v>
@@ -5039,7 +5093,7 @@
         <v>101</v>
       </c>
       <c r="F69" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G69" s="3" t="s">
         <v>77</v>
@@ -5067,6 +5121,12 @@
       </c>
       <c r="O69" s="3">
         <v>0</v>
+      </c>
+      <c r="P69" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q69" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="R69" s="3" t="s">
         <v>83</v>
@@ -5361,7 +5421,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>